<commit_message>
Many code changes performed
</commit_message>
<xml_diff>
--- a/src/main/java/com/naukri/qa/testdata/SearchTestData.xlsx
+++ b/src/main/java/com/naukri/qa/testdata/SearchTestData.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9A2AF5B1-C5F0-4C12-997C-9D07C058A26F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{381769B6-C627-44D4-955B-5DE353F3CCB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="23280" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="23304" windowHeight="13224" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:Q14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -377,7 +378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -409,4 +410,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5BF2E1-3E02-4DA3-97A5-960E956D4129}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>